<commit_message>
feat: update dragon config
</commit_message>
<xml_diff>
--- a/Excels/Dragon_龙表.xlsx
+++ b/Excels/Dragon_龙表.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>int</t>
   </si>
@@ -24,9 +24,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>bagId</t>
-  </si>
-  <si>
     <t>avatar</t>
   </si>
   <si>
@@ -51,15 +48,9 @@
     <t>cost</t>
   </si>
   <si>
-    <t>successRateAlgoId</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
-    <t xml:space="preserve">背包物 ID</t>
-  </si>
-  <si>
     <t>形象</t>
   </si>
   <si>
@@ -82,9 +73,6 @@
   </si>
   <si>
     <t>捕捉消耗</t>
-  </si>
-  <si>
-    <t>捕捉成功率算法</t>
   </si>
 </sst>
 </file>
@@ -122,11 +110,8 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -137,7 +122,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -145,11 +130,8 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,556 +646,502 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" style="1" width="10.875"/>
-    <col customWidth="1" min="3" max="3" width="33.625"/>
-    <col bestFit="1" customWidth="1" min="11" max="11" width="16.75"/>
-    <col customWidth="1" min="12" max="12" width="51.25"/>
-    <col customWidth="1" min="13" max="15" width="17.125"/>
+    <col customWidth="1" min="2" max="2" width="33.625"/>
+    <col customWidth="1" min="10" max="12" width="17.125"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" s="2" customFormat="1" ht="30">
-      <c r="A2" s="3" t="s">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" s="1" customFormat="1">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" s="2" customFormat="1">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" s="1" customFormat="1">
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" s="1" customFormat="1">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" s="4" customFormat="1">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" s="4" customFormat="1">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>300</v>
+      </c>
+      <c r="G5" s="4">
+        <v>80</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>10</v>
+      </c>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" s="4" customFormat="1">
+      <c r="A6" s="4">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
+        <v>300</v>
+      </c>
+      <c r="G6" s="4">
+        <v>80</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>10</v>
+      </c>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" s="4" customFormat="1">
+      <c r="A7" s="4">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>3</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>300</v>
+      </c>
+      <c r="G7" s="4">
+        <v>80</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>10</v>
+      </c>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" s="4" customFormat="1">
+      <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="B8" s="4">
         <v>0</v>
       </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="7">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="6">
+      <c r="C8" s="4">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
         <v>300</v>
       </c>
-      <c r="H5" s="1">
+      <c r="G8" s="4">
         <v>80</v>
       </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="H8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4">
         <v>10</v>
       </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>2</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5">
-        <v>1</v>
-      </c>
-      <c r="G6" s="6">
-        <v>300</v>
-      </c>
-      <c r="H6" s="1">
-        <v>80</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1">
-        <v>10</v>
-      </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1">
-      <c r="A7" s="1">
-        <v>3</v>
-      </c>
-      <c r="B7" s="5">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>3</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1</v>
-      </c>
-      <c r="G7" s="6">
-        <v>300</v>
-      </c>
-      <c r="H7" s="1">
-        <v>80</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1">
-        <v>10</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" s="1" customFormat="1">
-      <c r="A8" s="1">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>4</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
-        <v>300</v>
-      </c>
-      <c r="H8" s="1">
-        <v>80</v>
-      </c>
-      <c r="I8" s="1">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1">
-        <v>10</v>
-      </c>
-      <c r="K8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" s="1" customFormat="1"/>
-    <row r="10" s="1" customFormat="1">
-      <c r="B10" s="5"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" s="4" customFormat="1"/>
+    <row r="10" s="4" customFormat="1">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" s="1" customFormat="1">
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" s="4" customFormat="1">
+      <c r="C11" s="5"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" s="1" customFormat="1">
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" s="4" customFormat="1">
+      <c r="C12" s="5"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" s="1" customFormat="1">
-      <c r="B13" s="5"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="7"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" s="1" customFormat="1">
-      <c r="G14" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" s="4" customFormat="1">
+      <c r="B13" s="4"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="6"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" s="4" customFormat="1">
+      <c r="F14" s="5"/>
+      <c r="G14" s="7"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" s="1" customFormat="1">
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="6"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" s="4" customFormat="1">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="7"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-    </row>
-    <row r="16" s="1" customFormat="1">
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="6"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" s="4" customFormat="1">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="7"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="17" s="1" customFormat="1">
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="6"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+    </row>
+    <row r="17" s="4" customFormat="1">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="7"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" s="1" customFormat="1">
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-    </row>
-    <row r="19" s="1" customFormat="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="5"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="6"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" s="4" customFormat="1">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" s="4" customFormat="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="7"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-    </row>
-    <row r="20" s="1" customFormat="1">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="6"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" s="4" customFormat="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="7"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-    </row>
-    <row r="21" s="1" customFormat="1">
-      <c r="A21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" s="1" customFormat="1">
-      <c r="A22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" s="1" customFormat="1">
-      <c r="A23" s="6"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" s="1" customFormat="1">
-      <c r="A24" s="6"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" s="1" customFormat="1">
-      <c r="A25" s="6"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+    </row>
+    <row r="21" s="4" customFormat="1">
+      <c r="A21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" s="4" customFormat="1">
+      <c r="A22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" s="4" customFormat="1">
+      <c r="A23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" s="4" customFormat="1">
+      <c r="A24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" s="4" customFormat="1">
+      <c r="A25" s="5"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" s="1" customFormat="1">
-      <c r="A26" s="6"/>
-      <c r="B26" s="5"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" s="4" customFormat="1">
+      <c r="A26" s="5"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="6"/>
-    </row>
-    <row r="27" s="1" customFormat="1">
-      <c r="A27" s="6"/>
-      <c r="B27" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" s="4" customFormat="1">
+      <c r="A27" s="5"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="6"/>
-    </row>
-    <row r="28" s="1" customFormat="1">
-      <c r="A28" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" s="4" customFormat="1">
+      <c r="A28" s="5"/>
+      <c r="C28" s="5"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="6"/>
-    </row>
-    <row r="29" s="1" customFormat="1">
-      <c r="A29" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" s="4" customFormat="1">
+      <c r="A29" s="5"/>
+      <c r="C29" s="5"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="6"/>
-    </row>
-    <row r="30" s="1" customFormat="1">
-      <c r="A30" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" s="4" customFormat="1">
+      <c r="A30" s="5"/>
+      <c r="C30" s="5"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="6"/>
-    </row>
-    <row r="31" s="1" customFormat="1">
-      <c r="A31" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" s="4" customFormat="1">
+      <c r="A31" s="5"/>
+      <c r="C31" s="5"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="32" s="1" customFormat="1">
-      <c r="A32" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" s="4" customFormat="1">
+      <c r="A32" s="5"/>
+      <c r="C32" s="5"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="6"/>
-    </row>
-    <row r="33" s="1" customFormat="1">
-      <c r="A33" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" s="4" customFormat="1">
+      <c r="A33" s="5"/>
+      <c r="C33" s="5"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="6"/>
-    </row>
-    <row r="34" s="1" customFormat="1">
-      <c r="A34" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" s="4" customFormat="1">
+      <c r="A34" s="5"/>
+      <c r="C34" s="5"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="6"/>
-    </row>
-    <row r="35" s="1" customFormat="1">
-      <c r="A35" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" s="4" customFormat="1">
+      <c r="A35" s="5"/>
+      <c r="C35" s="5"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="6"/>
-    </row>
-    <row r="36" s="1" customFormat="1">
-      <c r="A36" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" s="4" customFormat="1">
+      <c r="A36" s="5"/>
+      <c r="C36" s="5"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="8"/>
-    </row>
-    <row r="37" s="1" customFormat="1">
-      <c r="A37" s="6"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" s="4" customFormat="1">
+      <c r="A37" s="5"/>
+      <c r="C37" s="5"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" s="1" customFormat="1">
-      <c r="A38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" s="1" customFormat="1">
-      <c r="A39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="9"/>
-    </row>
-    <row r="40" s="1" customFormat="1">
-      <c r="A40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="9"/>
-    </row>
-    <row r="41" s="1" customFormat="1">
-      <c r="A41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="9"/>
-    </row>
-    <row r="42" s="1" customFormat="1">
-      <c r="A42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="9"/>
-    </row>
-    <row r="43" s="1" customFormat="1">
-      <c r="A43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="9"/>
-    </row>
-    <row r="44" s="1" customFormat="1">
-      <c r="A44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="9"/>
-    </row>
-    <row r="45" s="1" customFormat="1"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" s="4" customFormat="1">
+      <c r="A38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" s="4" customFormat="1">
+      <c r="A39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" s="4" customFormat="1">
+      <c r="A40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" s="4" customFormat="1">
+      <c r="A41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" s="4" customFormat="1">
+      <c r="A42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" s="4" customFormat="1">
+      <c r="A43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" s="4" customFormat="1">
+      <c r="A44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" s="4" customFormat="1"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="1.0249999999999997" bottom="1.0249999999999997" header="0.78750000000000009" footer="0.78750000000000009"/>

</xml_diff>

<commit_message>
feat: update Dragon Res
同步龙娘角色资源
</commit_message>
<xml_diff>
--- a/Excels/Dragon_龙表.xlsx
+++ b/Excels/Dragon_龙表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MetaApp\Editor_Win64\MetaWorldSaved\Saved\MetaWorld\Project\Edit\DragonVerse\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MetaApp\Editor_Win64\MetaWorldSaved\Saved\MetaWorld\Project\Edit\DragonVerse\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3B3FE0-E9F9-4F0F-AF53-5764DF6738C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BEAC49-88DA-4355-9342-F3797002C22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>int</t>
   </si>
@@ -86,6 +86,22 @@
   </si>
   <si>
     <t>1|2|3|4|56|7|8|9|10|11|12</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>E6BC7E3C4AD0360A3871539DB8AD1C8C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3211A8204237F13B0F32058A52224938</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>9738674B4A58D76D124FFCBE4650659F</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>65F42892423491C2DA80E6AD3E9AD625</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -139,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -164,6 +180,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -395,14 +414,14 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="33.59765625" customWidth="1"/>
-    <col min="5" max="5" width="22.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="17.09765625" customWidth="1"/>
+    <col min="2" max="2" width="37.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="17.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -434,7 +453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -497,8 +516,8 @@
       <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="4">
-        <v>0</v>
+      <c r="B5" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -526,8 +545,8 @@
       <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="4">
-        <v>0</v>
+      <c r="B6" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="C6" s="5">
         <v>2</v>
@@ -555,8 +574,8 @@
       <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" s="4">
-        <v>0</v>
+      <c r="B7" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="C7" s="5">
         <v>3</v>
@@ -584,8 +603,8 @@
       <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="4">
-        <v>0</v>
+      <c r="B8" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="C8" s="4">
         <v>4</v>

</xml_diff>